<commit_message>
new numerators, and french level translation
</commit_message>
<xml_diff>
--- a/contextspecific/context_info.xlsx
+++ b/contextspecific/context_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/Analysis/MSNAEducation/contextspecific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="578" documentId="8_{0D5FD4D3-65A8-4B21-9AB8-E9E825B880B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E45A537A-8F10-4E7B-B5CD-43C58456DCAB}"/>
+  <xr:revisionPtr revIDLastSave="580" documentId="8_{0D5FD4D3-65A8-4B21-9AB8-E9E825B880B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA09220B-C360-4FD3-B76E-1A990419B88D}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="3" xr2:uid="{E7005411-AC04-408A-88F1-7D900FA9C136}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11265" activeTab="1" xr2:uid="{E7005411-AC04-408A-88F1-7D900FA9C136}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -828,18 +828,12 @@
     <t>level6</t>
   </si>
   <si>
-    <t>kindergarden, 4,3</t>
-  </si>
-  <si>
     <t>primary, 7, 8</t>
   </si>
   <si>
     <t>lower secondary, 15, 2</t>
   </si>
   <si>
-    <t>upper secondary, 17, 2</t>
-  </si>
-  <si>
     <t>level7</t>
   </si>
   <si>
@@ -853,6 +847,12 @@
   </si>
   <si>
     <t>august</t>
+  </si>
+  <si>
+    <t>écoles maternelles, 4,3</t>
+  </si>
+  <si>
+    <t>secondaire deuxième cycle, 17, 2</t>
   </si>
 </sst>
 </file>
@@ -1907,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED9E328-A731-4E3C-8AA8-F5577ADA7429}">
   <dimension ref="A1:K194"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2036,7 +2036,7 @@
         <v>82</v>
       </c>
       <c r="E14" s="103" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F14" s="4"/>
     </row>
@@ -2049,7 +2049,7 @@
         <v>83</v>
       </c>
       <c r="E15" s="103" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F15" s="4"/>
     </row>
@@ -2062,7 +2062,7 @@
         <v>84</v>
       </c>
       <c r="E16" s="103" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F16" s="4"/>
     </row>
@@ -2075,7 +2075,7 @@
         <v>85</v>
       </c>
       <c r="E17" s="103" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F17" s="4"/>
     </row>
@@ -2105,7 +2105,7 @@
       <c r="B20" s="5"/>
       <c r="C20" s="105"/>
       <c r="D20" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E20" s="103" t="s">
         <v>96</v>
@@ -2126,20 +2126,20 @@
         <v>92</v>
       </c>
       <c r="E22" s="103" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.75">
       <c r="B23" s="5"/>
       <c r="C23" s="94" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="F23" s="4"/>
     </row>
@@ -4008,7 +4008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BDDC9E-037F-4A19-9345-EA3F702B4B09}">
   <dimension ref="A1:K136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="B8" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>

</xml_diff>